<commit_message>
Papierformat an DIN-B-Reihe angelehnt
</commit_message>
<xml_diff>
--- a/test/Schriftgrößen.xlsx
+++ b/test/Schriftgrößen.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
   <si>
     <t>A4</t>
   </si>
@@ -65,15 +65,6 @@
     <t>Papierformat</t>
   </si>
   <si>
-    <t>7pt</t>
-  </si>
-  <si>
-    <t>8pt</t>
-  </si>
-  <si>
-    <t>6pt</t>
-  </si>
-  <si>
     <t>Spalten</t>
   </si>
   <si>
@@ -93,6 +84,54 @@
   </si>
   <si>
     <t>Größen für Ränder</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>D0</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>C0</t>
+  </si>
+  <si>
+    <t>B0</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>B6</t>
   </si>
 </sst>
 </file>
@@ -128,16 +167,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -419,340 +455,441 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" customWidth="1"/>
-    <col min="5" max="6" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" style="1" customWidth="1"/>
+    <col min="5" max="6" width="10.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="3"/>
+      <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="2"/>
       <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="B3" s="1">
         <v>12</v>
       </c>
-      <c r="C3">
-        <v>3.5</v>
+      <c r="C3" s="1">
+        <v>1.6</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
       </c>
       <c r="E3" s="1">
-        <v>10</v>
-      </c>
-      <c r="F3" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D4" s="1">
-        <v>2</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="1"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="1">
-        <v>13</v>
-      </c>
-      <c r="C5">
-        <v>2.5</v>
+        <v>34</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
       </c>
-      <c r="E5" s="1">
-        <v>11</v>
-      </c>
-      <c r="F5" s="1">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D6" s="1">
-        <v>2</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="1"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>10</v>
-      </c>
-      <c r="C7">
-        <v>3.5</v>
+        <v>28</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
       </c>
-      <c r="E7" s="1">
-        <v>12</v>
-      </c>
-      <c r="F7" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="D8" s="1">
-        <v>2</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="1"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="1">
-        <v>11</v>
-      </c>
-      <c r="C9">
-        <v>4.5</v>
+        <v>30</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
       </c>
-      <c r="E9" s="1">
-        <v>13</v>
-      </c>
-      <c r="F9" s="1">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="D10" s="1">
-        <v>2</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="1"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="D12" s="1">
-        <v>2</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="1">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="D14" s="1">
-        <v>2</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="1">
-        <v>10</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="D16" s="1">
-        <v>2</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="1">
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="1">
-        <v>1</v>
-      </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="D18" s="1">
-        <v>2</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="1">
-        <v>12</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="D20" s="1">
-        <v>2</v>
-      </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" s="1">
-        <v>13</v>
-      </c>
-      <c r="D21" s="1">
-        <v>1</v>
-      </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="D22" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="D24" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="1">
-        <v>10</v>
-      </c>
-      <c r="D23" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="D24" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="1">
-        <v>11</v>
-      </c>
-      <c r="D25" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="D26" s="1">
-        <v>2</v>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D36" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D42" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D43" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D46" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D48" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D49" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D50" s="1">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>